<commit_message>
Ready to fabricate with Sierra Circuits. (baring drill file and ODB++ pass inspection)
</commit_message>
<xml_diff>
--- a/OWLSAT Antenna PCB/Project Outputs for OWLSAT Antenna PCB/BOM/Bill of Materials-Antenna.xlsx
+++ b/OWLSAT Antenna PCB/Project Outputs for OWLSAT Antenna PCB/BOM/Bill of Materials-Antenna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\PCB\OWLSAT Antenna PCB\Project Outputs for OWLSAT Antenna PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F0F06CE-B4D6-468C-9B4B-950B65E04F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA9D150F-0121-4341-AC2D-D6740BD0BCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11325" xr2:uid="{47D655F6-FD71-49C9-8AE7-9D1711AC9F2A}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11325" xr2:uid="{85DB30C0-4888-4871-8B55-2A1FD06C22D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Antenna" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F43DD704-8D32-4147-9AB4-7A0B556D15E7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F95AFAE-6560-42A4-B66B-82DA6EEAC14A}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Fixed a clearance issue. Board spec'd at 00 for this configuration.
</commit_message>
<xml_diff>
--- a/OWLSAT Antenna PCB/Project Outputs for OWLSAT Antenna PCB/BOM/Bill of Materials-Antenna.xlsx
+++ b/OWLSAT Antenna PCB/Project Outputs for OWLSAT Antenna PCB/BOM/Bill of Materials-Antenna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\PCB\OWLSAT Antenna PCB\Project Outputs for OWLSAT Antenna PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA9D150F-0121-4341-AC2D-D6740BD0BCBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07F9552A-F775-40B0-BAD6-C01AC2AC63E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11325" xr2:uid="{85DB30C0-4888-4871-8B55-2A1FD06C22D3}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11325" xr2:uid="{2A042E26-F4E5-4767-A8F8-E869A60944DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Antenna" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F95AFAE-6560-42A4-B66B-82DA6EEAC14A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE482307-2641-4C4A-909B-71C2E8E34B2F}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Modified board to fit no-touch requirements at lowest cost for both Advanced Circuits and Sierra Circuits.
</commit_message>
<xml_diff>
--- a/OWLSAT Antenna PCB/Project Outputs for OWLSAT Antenna PCB/BOM/Bill of Materials-Antenna.xlsx
+++ b/OWLSAT Antenna PCB/Project Outputs for OWLSAT Antenna PCB/BOM/Bill of Materials-Antenna.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\PCB\OWLSAT Antenna PCB\Project Outputs for OWLSAT Antenna PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07F9552A-F775-40B0-BAD6-C01AC2AC63E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEF8A492-766E-4F6F-96D3-631207041F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11325" xr2:uid="{2A042E26-F4E5-4767-A8F8-E869A60944DE}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11325" xr2:uid="{C8927FCA-5C3D-40FE-95CB-6C941826CE86}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Antenna" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE482307-2641-4C4A-909B-71C2E8E34B2F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EC6CF7-55D2-4110-994D-304A9B84389E}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Sent for fabrication. Pre-fabrication documentation complete.
</commit_message>
<xml_diff>
--- a/OWLSAT Antenna PCB/Project Outputs for OWLSAT Antenna PCB/BOM/Bill of Materials-Antenna.xlsx
+++ b/OWLSAT Antenna PCB/Project Outputs for OWLSAT Antenna PCB/BOM/Bill of Materials-Antenna.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\james\Desktop\PCB\OWLSAT Antenna PCB\Project Outputs for OWLSAT Antenna PCB\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEF8A492-766E-4F6F-96D3-631207041F95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B481340-89A9-4628-BD79-D90B7E5BE407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11325" xr2:uid="{C8927FCA-5C3D-40FE-95CB-6C941826CE86}"/>
+    <workbookView xWindow="-24555" yWindow="2085" windowWidth="21600" windowHeight="11325" xr2:uid="{0B94667B-DF3C-4727-B9F6-F4A7EFB45A5B}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill of Materials-Antenna" sheetId="1" r:id="rId1"/>
@@ -482,7 +482,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04EC6CF7-55D2-4110-994D-304A9B84389E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9ABAD19-AB41-43C4-AB53-E1E72CAFDA6A}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>